<commit_message>
Add incorp, finish update
</commit_message>
<xml_diff>
--- a/DCE_update/inputs/inputs.xlsx
+++ b/DCE_update/inputs/inputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="28">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -49,7 +49,13 @@
     <t xml:space="preserve">man.ph</t>
   </si>
   <si>
-    <t xml:space="preserve">EF1</t>
+    <t xml:space="preserve">incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t.incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EF.report</t>
   </si>
   <si>
     <t xml:space="preserve">Cattle</t>
@@ -64,6 +70,9 @@
     <t xml:space="preserve">March</t>
   </si>
   <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
     <t xml:space="preserve">April</t>
   </si>
   <si>
@@ -83,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Trailing hose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep</t>
   </si>
   <si>
     <t xml:space="preserve">May</t>
@@ -106,6 +118,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -165,9 +178,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -187,24 +204,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
+      <selection pane="topLeft" activeCell="O33" activeCellId="0" sqref="O33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,22 +255,28 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>4.9</v>
@@ -267,7 +290,11 @@
       <c r="I2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="0" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -276,16 +303,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>8.5</v>
@@ -299,7 +326,11 @@
       <c r="I3" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="0" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -308,16 +339,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>4.9</v>
@@ -331,7 +362,11 @@
       <c r="I4" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="0" t="n">
         <v>12</v>
       </c>
     </row>
@@ -340,16 +375,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>8.5</v>
@@ -363,7 +398,11 @@
       <c r="I5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="0" t="n">
         <v>14</v>
       </c>
     </row>
@@ -372,16 +411,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>15.75</v>
@@ -395,7 +434,11 @@
       <c r="I6" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -404,16 +447,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>17.55</v>
@@ -427,7 +470,11 @@
       <c r="I7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="0" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -436,16 +483,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>14.6</v>
@@ -459,7 +506,11 @@
       <c r="I8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -468,16 +519,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>14.6</v>
@@ -491,7 +542,11 @@
       <c r="I9" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="0" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -500,16 +555,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>4.9</v>
@@ -523,8 +578,14 @@
       <c r="I10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>22</v>
+      <c r="J10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>3.1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,16 +593,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>8.5</v>
@@ -555,8 +616,14 @@
       <c r="I11" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J11" s="0" t="n">
-        <v>27</v>
+      <c r="J11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>4.7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,16 +631,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>4.9</v>
@@ -587,22 +654,29 @@
       <c r="I12" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="J12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="0" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>8.5</v>
@@ -615,6 +689,13 @@
       </c>
       <c r="I13" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="0" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,16 +703,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>12.4</v>
@@ -645,34 +726,48 @@
       <c r="I14" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="J14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>16.867</v>
+        <v>16.86667</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>3.182</v>
+        <v>3.1816667</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>6.5</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="0" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,28 +775,37 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>16.867</v>
+        <v>16.86667</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>3.182</v>
+        <v>3.1816667</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>6.5</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,16 +813,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>14.6</v>
@@ -731,6 +835,13 @@
       </c>
       <c r="I17" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,16 +849,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>14.6</v>
@@ -760,6 +871,15 @@
       </c>
       <c r="I18" s="0" t="n">
         <v>7</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>9.2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,16 +887,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>4.9</v>
@@ -790,7 +910,11 @@
       <c r="I19" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="0" t="n">
         <v>1.8</v>
       </c>
     </row>
@@ -799,16 +923,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>8.5</v>
@@ -822,7 +946,11 @@
       <c r="I20" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="0" t="n">
         <v>1.8</v>
       </c>
     </row>
@@ -831,16 +959,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>4.9</v>
@@ -854,7 +982,11 @@
       <c r="I21" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="0" t="n">
         <v>9.7</v>
       </c>
     </row>
@@ -863,16 +995,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>8.5</v>
@@ -886,7 +1018,11 @@
       <c r="I22" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="0" t="n">
         <v>9.8</v>
       </c>
     </row>
@@ -895,16 +1031,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>15.75</v>
@@ -918,7 +1054,11 @@
       <c r="I23" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="J23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -927,16 +1067,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>17.55</v>
@@ -950,7 +1090,11 @@
       <c r="I24" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="J24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="0" t="n">
         <v>1.8</v>
       </c>
     </row>
@@ -959,16 +1103,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>14.6</v>
@@ -982,7 +1126,11 @@
       <c r="I25" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="J25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -991,16 +1139,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>14.6</v>
@@ -1014,7 +1162,11 @@
       <c r="I26" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J26" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="0" t="n">
         <v>1.8</v>
       </c>
     </row>
@@ -1023,16 +1175,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>4.9</v>
@@ -1046,8 +1198,14 @@
       <c r="I27" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J27" s="0" t="n">
-        <v>14</v>
+      <c r="J27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,16 +1213,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>8.5</v>
@@ -1078,8 +1236,14 @@
       <c r="I28" s="0" t="n">
         <v>7.2</v>
       </c>
-      <c r="J28" s="0" t="n">
-        <v>15</v>
+      <c r="J28" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,16 +1251,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>4.9</v>
@@ -1109,6 +1273,13 @@
       </c>
       <c r="I29" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,16 +1287,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>8.5</v>
@@ -1138,6 +1309,13 @@
       </c>
       <c r="I30" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,16 +1323,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>12.4</v>
@@ -1167,6 +1345,13 @@
       </c>
       <c r="I31" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,28 +1359,35 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>16.867</v>
+        <v>16.86667</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>3.182</v>
+        <v>3.1816667</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>3.9</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,28 +1395,37 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>16.867</v>
+        <v>16.86667</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>3.182</v>
+        <v>3.1816667</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>3.9</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>6.7</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,16 +1433,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>14.6</v>
@@ -1254,6 +1455,13 @@
       </c>
       <c r="I34" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,16 +1469,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>14.6</v>
@@ -1283,6 +1491,15 @@
       </c>
       <c r="I35" s="0" t="n">
         <v>7.2</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L35" s="0" t="n">
+        <v>5.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>